<commit_message>
reading material added: control flow
</commit_message>
<xml_diff>
--- a/src/main/java/org/dia/_syllabus/course_details.xlsx
+++ b/src/main/java/org/dia/_syllabus/course_details.xlsx
@@ -298,7 +298,7 @@
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -361,7 +361,7 @@
         <v>44261</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
       <c r="B4" s="7" t="n">
         <f aca="false">B3+1</f>
@@ -377,7 +377,7 @@
         <v>44268</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
       <c r="B5" s="7" t="n">
         <f aca="false">B4+1</f>
@@ -389,7 +389,9 @@
       <c r="D5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9" t="n">
+        <v>44289</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>

</xml_diff>